<commit_message>
New files into develop branch
</commit_message>
<xml_diff>
--- a/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
+++ b/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\EoCEDwEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\EoCEDwEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,15 +32,6 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>Price Responsiveness in the AEO 2003 NEMS Residential and Commercial Buildings Sector Models</t>
-  </si>
-  <si>
-    <t>http://www.eia.gov/oiaf/analysispaper/elasticity/pdf/tbl.pdf</t>
-  </si>
-  <si>
-    <t>Page 1, Table 1</t>
-  </si>
-  <si>
     <t>This is a subset of Table 1 that includes only values from AEO2003 (not AEO99).</t>
   </si>
   <si>
@@ -98,21 +89,12 @@
     <t>Note:</t>
   </si>
   <si>
-    <t>We use same-price, long-run elasticities minus the 1-year short-run elasticities.</t>
-  </si>
-  <si>
-    <t>We calculate it this way because we assume that 1-year elasticities primarily reflect behavior</t>
-  </si>
-  <si>
     <t>change rather than equipment change, and the response of behavior to price per unit service</t>
   </si>
   <si>
     <t>provided (that is, controlling for things like efficiency of equipment) should be constant at</t>
   </si>
   <si>
-    <t>all timescales.  So, the portion of the long-run elasticitiy represented by the 1-year elasticity</t>
-  </si>
-  <si>
     <t>is still behavior change, and the rest is equipment efficiency change, which is what we are</t>
   </si>
   <si>
@@ -180,6 +162,24 @@
   </si>
   <si>
     <t>Elasticity by Fuel (dimensionless)</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/analysis/studies/buildings/energyuse/pdf/price_elasticities.pdf</t>
+  </si>
+  <si>
+    <t>Price Elasticities for Energy Use in Buildings of the United States</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>We use same-price, long-run elasticities minus the 3-year short-run elasticities.</t>
+  </si>
+  <si>
+    <t>We calculate it this way because we assume that 3-year elasticities primarily reflect behavior</t>
+  </si>
+  <si>
+    <t>all timescales.  So, the portion of the long-run elasticitiy represented by the 3-year elasticity</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -734,129 +736,129 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -872,7 +874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -887,17 +891,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -909,57 +913,57 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7">
-        <v>-0.2</v>
+        <v>-0.12</v>
       </c>
       <c r="C7" s="8">
-        <v>-0.28999999999999998</v>
+        <v>-0.21</v>
       </c>
       <c r="D7" s="9">
-        <v>-0.34</v>
+        <v>-0.25</v>
       </c>
       <c r="E7" s="7">
-        <v>-0.49</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="F7" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <v>0</v>
@@ -967,53 +971,53 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C8" s="8">
-        <v>-0.24</v>
+        <v>-0.13</v>
       </c>
       <c r="D8" s="9">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
       <c r="E8" s="7">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="F8" s="19">
-        <v>-0.41</v>
+        <v>-0.21</v>
       </c>
       <c r="G8" s="9">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10">
-        <v>-0.15</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C9" s="11">
-        <v>-0.27</v>
+        <v>-0.12</v>
       </c>
       <c r="D9" s="12">
-        <v>-0.34</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="E9" s="10">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F9" s="11">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G9" s="12">
-        <v>-0.6</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1025,57 +1029,57 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="G13" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="C14" s="8">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="D14" s="9">
-        <v>-0.2</v>
+        <v>-0.22</v>
       </c>
       <c r="E14" s="7">
-        <v>-0.45</v>
+        <v>-0.33</v>
       </c>
       <c r="F14" s="19">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
@@ -1083,48 +1087,48 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-0.15</v>
       </c>
       <c r="C15" s="8">
-        <v>-0.24</v>
+        <v>-0.25</v>
       </c>
       <c r="D15" s="9">
-        <v>-0.28999999999999998</v>
+        <v>-0.3</v>
       </c>
       <c r="E15" s="7">
-        <v>0.86</v>
+        <v>0.15</v>
       </c>
       <c r="F15" s="19">
-        <v>-0.4</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="G15" s="9">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10">
-        <v>-0.13</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="C16" s="11">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="D16" s="12">
-        <v>-0.28000000000000003</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="E16" s="10">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="F16" s="11">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="G16" s="12">
-        <v>-0.39</v>
+        <v>-0.42</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1143,9 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1150,89 +1156,89 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="24">
-        <f>'EIA Table 1'!E7-'EIA Table 1'!B7</f>
-        <v>-0.28999999999999998</v>
+        <f>'EIA Table 1'!E7-'EIA Table 1'!D7</f>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="C2" s="24">
         <f>B2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="D2" s="24">
-        <f>'EIA Table 1'!E14-'EIA Table 1'!B14</f>
-        <v>-0.35</v>
+        <f>'EIA Table 1'!E14-'EIA Table 1'!D14</f>
+        <v>-0.11000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C6" si="0">B3</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D3" s="23">
         <f>D5</f>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="24">
-        <f>'EIA Table 1'!F8-'EIA Table 1'!B8</f>
-        <v>-0.26999999999999996</v>
+        <f>'EIA Table 1'!F8-'EIA Table 1'!D8</f>
+        <v>-0.06</v>
       </c>
       <c r="C4" s="24">
         <f t="shared" si="0"/>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="D4" s="24">
-        <f>'EIA Table 1'!F15-'EIA Table 1'!B15</f>
-        <v>-0.26</v>
+        <f>'EIA Table 1'!F15-'EIA Table 1'!D15</f>
+        <v>-0.27999999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="24">
-        <f>'EIA Table 1'!G9-'EIA Table 1'!B9</f>
-        <v>-0.44999999999999996</v>
+        <f>'EIA Table 1'!G9-'EIA Table 1'!D9</f>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C5" s="24">
         <f t="shared" si="0"/>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D5" s="24">
-        <f>'EIA Table 1'!G16-'EIA Table 1'!B16</f>
-        <v>-0.26</v>
+        <f>'EIA Table 1'!G16-'EIA Table 1'!D16</f>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1247,7 +1253,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1261,70 +1267,70 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B8" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" ref="C8:D8" si="1">C5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D8" s="23">
         <f t="shared" si="1"/>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B9" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" ref="C9:D9" si="2">C5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" si="2"/>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B10" s="23">
         <f>B4</f>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" ref="C10:D10" si="3">C4</f>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="D10" s="23">
         <f t="shared" si="3"/>
-        <v>-0.26</v>
+        <v>-0.27999999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" s="23">
         <f>B2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" ref="C11:D11" si="4">C2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="D11" s="23">
         <f t="shared" si="4"/>
-        <v>-0.35</v>
+        <v>-0.11000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Jun's files 10.21
</commit_message>
<xml_diff>
--- a/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
+++ b/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\EoCEDwEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\EoCEDwEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,15 +32,6 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>Price Responsiveness in the AEO 2003 NEMS Residential and Commercial Buildings Sector Models</t>
-  </si>
-  <si>
-    <t>http://www.eia.gov/oiaf/analysispaper/elasticity/pdf/tbl.pdf</t>
-  </si>
-  <si>
-    <t>Page 1, Table 1</t>
-  </si>
-  <si>
     <t>This is a subset of Table 1 that includes only values from AEO2003 (not AEO99).</t>
   </si>
   <si>
@@ -98,21 +89,12 @@
     <t>Note:</t>
   </si>
   <si>
-    <t>We use same-price, long-run elasticities minus the 1-year short-run elasticities.</t>
-  </si>
-  <si>
-    <t>We calculate it this way because we assume that 1-year elasticities primarily reflect behavior</t>
-  </si>
-  <si>
     <t>change rather than equipment change, and the response of behavior to price per unit service</t>
   </si>
   <si>
     <t>provided (that is, controlling for things like efficiency of equipment) should be constant at</t>
   </si>
   <si>
-    <t>all timescales.  So, the portion of the long-run elasticitiy represented by the 1-year elasticity</t>
-  </si>
-  <si>
     <t>is still behavior change, and the rest is equipment efficiency change, which is what we are</t>
   </si>
   <si>
@@ -180,6 +162,24 @@
   </si>
   <si>
     <t>Elasticity by Fuel (dimensionless)</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/analysis/studies/buildings/energyuse/pdf/price_elasticities.pdf</t>
+  </si>
+  <si>
+    <t>Price Elasticities for Energy Use in Buildings of the United States</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>We use same-price, long-run elasticities minus the 3-year short-run elasticities.</t>
+  </si>
+  <si>
+    <t>We calculate it this way because we assume that 3-year elasticities primarily reflect behavior</t>
+  </si>
+  <si>
+    <t>all timescales.  So, the portion of the long-run elasticitiy represented by the 3-year elasticity</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -734,129 +736,129 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -872,7 +874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -887,17 +891,17 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -909,57 +913,57 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7">
-        <v>-0.2</v>
+        <v>-0.12</v>
       </c>
       <c r="C7" s="8">
-        <v>-0.28999999999999998</v>
+        <v>-0.21</v>
       </c>
       <c r="D7" s="9">
-        <v>-0.34</v>
+        <v>-0.25</v>
       </c>
       <c r="E7" s="7">
-        <v>-0.49</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="F7" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <v>0</v>
@@ -967,53 +971,53 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C8" s="8">
-        <v>-0.24</v>
+        <v>-0.13</v>
       </c>
       <c r="D8" s="9">
-        <v>-0.3</v>
+        <v>-0.15</v>
       </c>
       <c r="E8" s="7">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="F8" s="19">
-        <v>-0.41</v>
+        <v>-0.21</v>
       </c>
       <c r="G8" s="9">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10">
-        <v>-0.15</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C9" s="11">
-        <v>-0.27</v>
+        <v>-0.12</v>
       </c>
       <c r="D9" s="12">
-        <v>-0.34</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="E9" s="10">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F9" s="11">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G9" s="12">
-        <v>-0.6</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1025,57 +1029,57 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="G13" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="C14" s="8">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="D14" s="9">
-        <v>-0.2</v>
+        <v>-0.22</v>
       </c>
       <c r="E14" s="7">
-        <v>-0.45</v>
+        <v>-0.33</v>
       </c>
       <c r="F14" s="19">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
@@ -1083,48 +1087,48 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="7">
-        <v>-0.14000000000000001</v>
+        <v>-0.15</v>
       </c>
       <c r="C15" s="8">
-        <v>-0.24</v>
+        <v>-0.25</v>
       </c>
       <c r="D15" s="9">
-        <v>-0.28999999999999998</v>
+        <v>-0.3</v>
       </c>
       <c r="E15" s="7">
-        <v>0.86</v>
+        <v>0.15</v>
       </c>
       <c r="F15" s="19">
-        <v>-0.4</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="G15" s="9">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10">
-        <v>-0.13</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="C16" s="11">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="D16" s="12">
-        <v>-0.28000000000000003</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="E16" s="10">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="F16" s="11">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="G16" s="12">
-        <v>-0.39</v>
+        <v>-0.42</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1143,9 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1150,89 +1156,89 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="24">
-        <f>'EIA Table 1'!E7-'EIA Table 1'!B7</f>
-        <v>-0.28999999999999998</v>
+        <f>'EIA Table 1'!E7-'EIA Table 1'!D7</f>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="C2" s="24">
         <f>B2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="D2" s="24">
-        <f>'EIA Table 1'!E14-'EIA Table 1'!B14</f>
-        <v>-0.35</v>
+        <f>'EIA Table 1'!E14-'EIA Table 1'!D14</f>
+        <v>-0.11000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C6" si="0">B3</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D3" s="23">
         <f>D5</f>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="24">
-        <f>'EIA Table 1'!F8-'EIA Table 1'!B8</f>
-        <v>-0.26999999999999996</v>
+        <f>'EIA Table 1'!F8-'EIA Table 1'!D8</f>
+        <v>-0.06</v>
       </c>
       <c r="C4" s="24">
         <f t="shared" si="0"/>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="D4" s="24">
-        <f>'EIA Table 1'!F15-'EIA Table 1'!B15</f>
-        <v>-0.26</v>
+        <f>'EIA Table 1'!F15-'EIA Table 1'!D15</f>
+        <v>-0.27999999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="24">
-        <f>'EIA Table 1'!G9-'EIA Table 1'!B9</f>
-        <v>-0.44999999999999996</v>
+        <f>'EIA Table 1'!G9-'EIA Table 1'!D9</f>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C5" s="24">
         <f t="shared" si="0"/>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D5" s="24">
-        <f>'EIA Table 1'!G16-'EIA Table 1'!B16</f>
-        <v>-0.26</v>
+        <f>'EIA Table 1'!G16-'EIA Table 1'!D16</f>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1247,7 +1253,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1261,70 +1267,70 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B8" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" ref="C8:D8" si="1">C5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D8" s="23">
         <f t="shared" si="1"/>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B9" s="23">
         <f>B5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" ref="C9:D9" si="2">C5</f>
-        <v>-0.44999999999999996</v>
+        <v>-7.9999999999999988E-2</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" si="2"/>
-        <v>-0.26</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B10" s="23">
         <f>B4</f>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" ref="C10:D10" si="3">C4</f>
-        <v>-0.26999999999999996</v>
+        <v>-0.06</v>
       </c>
       <c r="D10" s="23">
         <f t="shared" si="3"/>
-        <v>-0.26</v>
+        <v>-0.27999999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" s="23">
         <f>B2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" ref="C11:D11" si="4">C2</f>
-        <v>-0.28999999999999998</v>
+        <v>-3.0000000000000027E-2</v>
       </c>
       <c r="D11" s="23">
         <f t="shared" si="4"/>
-        <v>-0.35</v>
+        <v>-0.11000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>